<commit_message>
🚧 Working on xslx
</commit_message>
<xml_diff>
--- a/app/app/data2.xlsx
+++ b/app/app/data2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BOG-A404-E-005\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook-ivan/Documents/uniminuto/BigData/app/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B115A1-A646-C449-85AF-89BCCDD9FC20}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="62">
   <si>
     <t>V-P</t>
   </si>
@@ -35,15 +36,9 @@
     <t>Mes</t>
   </si>
   <si>
-    <t># Mes</t>
-  </si>
-  <si>
     <t>Doc</t>
   </si>
   <si>
-    <t>Tipo Doc</t>
-  </si>
-  <si>
     <t>Zona</t>
   </si>
   <si>
@@ -56,9 +51,6 @@
     <t>Cliente</t>
   </si>
   <si>
-    <t>Producto Familia</t>
-  </si>
-  <si>
     <t>Pres</t>
   </si>
   <si>
@@ -74,9 +66,6 @@
     <t>kg-ltrs</t>
   </si>
   <si>
-    <t>Venta Neta $</t>
-  </si>
-  <si>
     <t>VTAS</t>
   </si>
   <si>
@@ -213,14 +202,23 @@
   </si>
   <si>
     <t>Cooperativa De Caficultores De Andes Ltda.</t>
+  </si>
+  <si>
+    <t>Producto-Familia</t>
+  </si>
+  <si>
+    <t>venta_neta</t>
+  </si>
+  <si>
+    <t>Tipo_doc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -302,7 +300,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -323,10 +321,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Millares [0]" xfId="1" builtinId="6"/>
+    <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -604,16 +602,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:Q21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -624,51 +620,51 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="Q1" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B2" s="6">
         <v>2014</v>
@@ -683,31 +679,27 @@
         <v>235989</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="6">
+        <v>1</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="6">
-        <v>900473575</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="6">
-        <v>1</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="O2" s="8">
         <v>10</v>
@@ -719,9 +711,9 @@
         <v>24.3</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B3" s="6">
         <v>2014</v>
@@ -736,31 +728,29 @@
         <v>235926</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>19</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H3" s="6"/>
       <c r="I3" s="6">
         <v>900473575</v>
       </c>
       <c r="J3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="L3" s="6">
         <v>25</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="O3" s="8">
         <v>2</v>
@@ -772,9 +762,9 @@
         <v>202.5</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B4" s="6">
         <v>2014</v>
@@ -789,31 +779,31 @@
         <v>235926</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I4" s="6">
         <v>900473575</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="L4" s="6">
         <v>25</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="O4" s="8">
         <v>1</v>
@@ -825,9 +815,9 @@
         <v>78.974999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B5" s="6">
         <v>2014</v>
@@ -842,31 +832,31 @@
         <v>235926</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I5" s="6">
         <v>900473575</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L5" s="6">
         <v>25</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="O5" s="8">
         <v>1</v>
@@ -878,9 +868,9 @@
         <v>53.298000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B6" s="6">
         <v>2014</v>
@@ -895,31 +885,31 @@
         <v>235926</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I6" s="6">
         <v>900473575</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L6" s="6">
         <v>25</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="O6" s="8">
         <v>2</v>
@@ -931,9 +921,9 @@
         <v>199.26</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B7" s="6">
         <v>2014</v>
@@ -948,31 +938,31 @@
         <v>235926</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I7" s="6">
         <v>900473575</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L7" s="6">
         <v>1</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="O7" s="8">
         <v>3</v>
@@ -984,9 +974,9 @@
         <v>44.954999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B8" s="6">
         <v>2014</v>
@@ -1001,31 +991,31 @@
         <v>235926</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I8" s="6">
         <v>900473575</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L8" s="6">
         <v>1</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="O8" s="8">
         <v>3</v>
@@ -1037,9 +1027,9 @@
         <v>71.189850000000007</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9" s="6">
         <v>2014</v>
@@ -1054,31 +1044,31 @@
         <v>235926</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I9" s="6">
         <v>900473575</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="L9" s="6">
         <v>1</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="O9" s="8">
         <v>3</v>
@@ -1090,9 +1080,9 @@
         <v>34.020000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B10" s="6">
         <v>2014</v>
@@ -1107,31 +1097,31 @@
         <v>235926</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I10" s="6">
         <v>900473575</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L10" s="6">
         <v>1</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O10" s="8">
         <v>3</v>
@@ -1143,9 +1133,9 @@
         <v>50.058</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B11" s="6">
         <v>2014</v>
@@ -1160,31 +1150,31 @@
         <v>235926</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I11" s="6">
         <v>900473575</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="L11" s="6">
         <v>1</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O11" s="8">
         <v>3</v>
@@ -1196,9 +1186,9 @@
         <v>119.07</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B12" s="6">
         <v>2014</v>
@@ -1213,31 +1203,31 @@
         <v>24506</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I12" s="6">
         <v>900473575</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="L12" s="6">
         <v>1</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O12" s="8">
         <v>-1</v>
@@ -1249,9 +1239,9 @@
         <v>-89.854110000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B13" s="6">
         <v>2014</v>
@@ -1266,31 +1256,31 @@
         <v>235949</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I13" s="6">
         <v>900473575</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="L13" s="6">
         <v>1</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O13" s="8">
         <v>1</v>
@@ -1302,9 +1292,9 @@
         <v>89.854110000000006</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B14" s="6">
         <v>2014</v>
@@ -1319,31 +1309,31 @@
         <v>235928</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I14" s="6">
         <v>900473575</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="L14" s="6">
         <v>200</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O14" s="8">
         <v>4</v>
@@ -1355,9 +1345,9 @@
         <v>6534.1121499999999</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B15" s="6">
         <v>2014</v>
@@ -1372,31 +1362,31 @@
         <v>235926</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I15" s="6">
         <v>900473575</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="L15" s="6">
         <v>4</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="O15" s="8">
         <v>3</v>
@@ -1408,9 +1398,9 @@
         <v>101.62260000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B16" s="6">
         <v>2014</v>
@@ -1425,31 +1415,31 @@
         <v>411675</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="L16" s="6">
         <v>20</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="N16" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="O16" s="8">
         <v>30</v>
@@ -1461,9 +1451,9 @@
         <v>1676.7</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B17" s="6">
         <v>2014</v>
@@ -1478,31 +1468,31 @@
         <v>411688</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I17" s="6">
         <v>70953633</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="L17" s="6">
         <v>20</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="N17" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="O17" s="8">
         <v>5</v>
@@ -1514,9 +1504,9 @@
         <v>293.25</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B18" s="6">
         <v>2014</v>
@@ -1531,31 +1521,31 @@
         <v>24343</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I18" s="6">
         <v>21460849</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L18" s="6">
         <v>20</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N18" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="O18" s="8">
         <v>-10</v>
@@ -1567,9 +1557,9 @@
         <v>-289</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B19" s="6">
         <v>2014</v>
@@ -1584,31 +1574,31 @@
         <v>24435</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I19" s="6">
         <v>890907638</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L19" s="6">
         <v>20</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N19" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="O19" s="8">
         <v>-50</v>
@@ -1620,9 +1610,9 @@
         <v>-1411</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B20" s="6">
         <v>2014</v>
@@ -1637,31 +1627,31 @@
         <v>411565</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I20" s="6">
         <v>21460849</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L20" s="6">
         <v>20</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N20" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="O20" s="8">
         <v>10</v>
@@ -1673,9 +1663,9 @@
         <v>289</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B21" s="6">
         <v>2014</v>
@@ -1690,31 +1680,31 @@
         <v>411569</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I21" s="6">
         <v>21460849</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L21" s="6">
         <v>20</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N21" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="O21" s="8">
         <v>10</v>

</xml_diff>